<commit_message>
Site Page with Button switch and Donut V1
</commit_message>
<xml_diff>
--- a/public_html/Randomdata.xlsx
+++ b/public_html/Randomdata.xlsx
@@ -110,7 +110,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -150,13 +150,15 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -442,18 +444,18 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
@@ -500,33 +502,33 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <f ca="1">RANDBETWEEN(5,100)</f>
-        <v>92</v>
-      </c>
-      <c r="C3" s="4">
+        <v>55</v>
+      </c>
+      <c r="C3" s="7">
         <f ca="1">RANDBETWEEN(10,15)/100</f>
-        <v>0.15</v>
-      </c>
-      <c r="D3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D3" s="5">
         <f ca="1">RANDBETWEEN(6,15)</f>
-        <v>15</v>
-      </c>
-      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="E3" s="5">
         <f ca="1">B3*$C$1*$K$4</f>
-        <v>119356.75200000001</v>
-      </c>
-      <c r="F3" s="3">
+        <v>71354.58</v>
+      </c>
+      <c r="F3" s="6">
         <f ca="1">B3*$C3*$K$4</f>
-        <v>120887.99999999999</v>
-      </c>
-      <c r="G3" s="2">
+        <v>67452.000000000015</v>
+      </c>
+      <c r="G3" s="6">
         <f t="shared" ref="G3:G17" ca="1" si="0">E3*D3</f>
-        <v>1790351.28</v>
-      </c>
-      <c r="H3" s="2">
+        <v>570836.64</v>
+      </c>
+      <c r="H3" s="6">
         <f ca="1">F3*D3</f>
-        <v>1813319.9999999998</v>
+        <v>539616.00000000012</v>
       </c>
       <c r="J3" t="s">
         <v>25</v>
@@ -539,33 +541,33 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <f t="shared" ref="B4:B17" ca="1" si="1">RANDBETWEEN(5,100)</f>
-        <v>10</v>
-      </c>
-      <c r="C4" s="4">
+        <v>19</v>
+      </c>
+      <c r="C4" s="7">
         <f t="shared" ref="C4:C17" ca="1" si="2">RANDBETWEEN(10,15)/100</f>
-        <v>0.1</v>
-      </c>
-      <c r="D4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D4" s="5">
         <f t="shared" ref="D4:D17" ca="1" si="3">RANDBETWEEN(6,15)</f>
         <v>11</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <f t="shared" ref="E4:E17" ca="1" si="4">B4*$C$1*$K$4</f>
-        <v>12973.560000000001</v>
-      </c>
-      <c r="F4" s="3">
+        <v>24649.764000000003</v>
+      </c>
+      <c r="F4" s="6">
         <f t="shared" ref="F4:F17" ca="1" si="5">B4*$C4*$K$4</f>
-        <v>8760</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>142709.16</v>
-      </c>
-      <c r="H4" s="2">
+        <v>23301.600000000002</v>
+      </c>
+      <c r="G4" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>271147.40400000004</v>
+      </c>
+      <c r="H4" s="6">
         <f t="shared" ref="H4:H17" ca="1" si="6">F4*D4</f>
-        <v>96360</v>
+        <v>256317.60000000003</v>
       </c>
       <c r="K4">
         <f>K3*K2</f>
@@ -576,101 +578,101 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
-        <f t="shared" ca="1" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="C5" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="D5">
-        <f t="shared" ca="1" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <f t="shared" ca="1" si="4"/>
-        <v>35028.612000000001</v>
-      </c>
-      <c r="F5" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>33112.800000000003</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>490400.56800000003</v>
-      </c>
-      <c r="H5" s="2">
-        <f t="shared" ca="1" si="6"/>
-        <v>463579.20000000007</v>
+      <c r="B5" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="C5" s="7">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.15</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" ca="1" si="4"/>
+        <v>72651.936000000016</v>
+      </c>
+      <c r="F5" s="6">
+        <f t="shared" ca="1" si="5"/>
+        <v>73584</v>
+      </c>
+      <c r="G5" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>435911.6160000001</v>
+      </c>
+      <c r="H5" s="6">
+        <f t="shared" ca="1" si="6"/>
+        <v>441504</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
-        <f t="shared" ca="1" si="1"/>
-        <v>76</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="B6" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="C6" s="7">
         <f t="shared" ca="1" si="2"/>
         <v>0.14000000000000001</v>
       </c>
-      <c r="D6">
-        <f t="shared" ca="1" si="3"/>
-        <v>11</v>
-      </c>
-      <c r="E6">
-        <f t="shared" ca="1" si="4"/>
-        <v>98599.056000000011</v>
-      </c>
-      <c r="F6" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>93206.400000000009</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1084589.6160000002</v>
-      </c>
-      <c r="H6" s="2">
-        <f t="shared" ca="1" si="6"/>
-        <v>1025270.4000000001</v>
+      <c r="D6" s="5">
+        <f t="shared" ca="1" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" ca="1" si="4"/>
+        <v>84328.14</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" ca="1" si="5"/>
+        <v>79716.000000000015</v>
+      </c>
+      <c r="G6" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>674625.12</v>
+      </c>
+      <c r="H6" s="6">
+        <f t="shared" ca="1" si="6"/>
+        <v>637728.00000000012</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
-        <f t="shared" ca="1" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="C7" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.12</v>
-      </c>
-      <c r="D7">
-        <f t="shared" ca="1" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="E7">
-        <f t="shared" ca="1" si="4"/>
-        <v>23352.407999999999</v>
-      </c>
-      <c r="F7" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>18921.600000000002</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>186819.264</v>
-      </c>
-      <c r="H7" s="2">
-        <f t="shared" ca="1" si="6"/>
-        <v>151372.80000000002</v>
-      </c>
-      <c r="M7" s="5">
+      <c r="B7" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="C7" s="7">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" ca="1" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" ca="1" si="4"/>
+        <v>108977.90400000001</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" ca="1" si="5"/>
+        <v>73584</v>
+      </c>
+      <c r="G7" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1634668.56</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" ca="1" si="6"/>
+        <v>1103760</v>
+      </c>
+      <c r="M7" s="4">
         <f ca="1">RANDBETWEEN(0.1,0.15)</f>
         <v>1</v>
       </c>
@@ -679,348 +681,348 @@
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
-        <f t="shared" ca="1" si="1"/>
-        <v>82</v>
-      </c>
-      <c r="C8" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.13</v>
-      </c>
-      <c r="D8">
-        <f t="shared" ca="1" si="3"/>
-        <v>11</v>
-      </c>
-      <c r="E8">
-        <f t="shared" ca="1" si="4"/>
-        <v>106383.19200000001</v>
-      </c>
-      <c r="F8" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>93381.6</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1170215.1120000002</v>
-      </c>
-      <c r="H8" s="2">
-        <f t="shared" ca="1" si="6"/>
-        <v>1027197.6000000001</v>
+      <c r="B8" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="C8" s="7">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" ca="1" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" ca="1" si="4"/>
+        <v>120654.10800000001</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" ca="1" si="5"/>
+        <v>114055.20000000001</v>
+      </c>
+      <c r="G8" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1689157.5120000001</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" ca="1" si="6"/>
+        <v>1596772.8000000003</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9">
-        <f t="shared" ca="1" si="1"/>
-        <v>63</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="B9" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C9" s="7">
         <f t="shared" ca="1" si="2"/>
         <v>0.11</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="5">
         <f t="shared" ca="1" si="3"/>
         <v>6</v>
       </c>
-      <c r="E9">
-        <f t="shared" ca="1" si="4"/>
-        <v>81733.428000000014</v>
-      </c>
-      <c r="F9" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>60706.799999999996</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>490400.56800000009</v>
-      </c>
-      <c r="H9" s="2">
-        <f t="shared" ca="1" si="6"/>
-        <v>364240.8</v>
+      <c r="E9" s="5">
+        <f t="shared" ca="1" si="4"/>
+        <v>16865.628000000001</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" ca="1" si="5"/>
+        <v>12526.8</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>101193.76800000001</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" ca="1" si="6"/>
+        <v>75160.799999999988</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B10">
-        <f t="shared" ca="1" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="C10" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="D10">
+      <c r="B10" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.13</v>
+      </c>
+      <c r="D10" s="5">
         <f ca="1">RANDBETWEEN(6,15)</f>
-        <v>10</v>
-      </c>
-      <c r="E10">
-        <f t="shared" ca="1" si="4"/>
-        <v>12973.560000000001</v>
-      </c>
-      <c r="F10" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>8760</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>129735.6</v>
-      </c>
-      <c r="H10" s="2">
-        <f t="shared" ca="1" si="6"/>
-        <v>87600</v>
+        <v>12</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" ca="1" si="4"/>
+        <v>70057.224000000002</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" ca="1" si="5"/>
+        <v>61495.200000000004</v>
+      </c>
+      <c r="G10" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>840686.68800000008</v>
+      </c>
+      <c r="H10" s="6">
+        <f t="shared" ca="1" si="6"/>
+        <v>737942.4</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11">
-        <f t="shared" ca="1" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="C11" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="D11">
-        <f t="shared" ca="1" si="3"/>
+      <c r="B11" s="5">
+        <f t="shared" ca="1" si="1"/>
         <v>11</v>
       </c>
-      <c r="E11">
-        <f t="shared" ca="1" si="4"/>
-        <v>58381.020000000004</v>
-      </c>
-      <c r="F11" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>39420</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>642191.22000000009</v>
-      </c>
-      <c r="H11" s="2">
-        <f t="shared" ca="1" si="6"/>
-        <v>433620</v>
+      <c r="C11" s="7">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" ca="1" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" ca="1" si="4"/>
+        <v>14270.916000000001</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" ca="1" si="5"/>
+        <v>13490.4</v>
+      </c>
+      <c r="G11" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>185521.90800000002</v>
+      </c>
+      <c r="H11" s="6">
+        <f t="shared" ca="1" si="6"/>
+        <v>175375.19999999998</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B12">
-        <f t="shared" ca="1" si="1"/>
-        <v>83</v>
-      </c>
-      <c r="C12" s="4">
+      <c r="B12" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="C12" s="7">
         <f t="shared" ca="1" si="2"/>
         <v>0.15</v>
       </c>
-      <c r="D12">
-        <f t="shared" ca="1" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="E12">
-        <f t="shared" ca="1" si="4"/>
-        <v>107680.54800000001</v>
-      </c>
-      <c r="F12" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>109062</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1292166.5760000001</v>
-      </c>
-      <c r="H12" s="2">
-        <f t="shared" ca="1" si="6"/>
-        <v>1308744</v>
+      <c r="D12" s="5">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" ca="1" si="4"/>
+        <v>32433.9</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" ca="1" si="5"/>
+        <v>32850</v>
+      </c>
+      <c r="G12" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>291905.10000000003</v>
+      </c>
+      <c r="H12" s="6">
+        <f t="shared" ca="1" si="6"/>
+        <v>295650</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13">
-        <f t="shared" ca="1" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="C13" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="D13">
-        <f t="shared" ca="1" si="3"/>
-        <v>13</v>
-      </c>
-      <c r="E13">
-        <f t="shared" ca="1" si="4"/>
-        <v>77841.360000000015</v>
-      </c>
-      <c r="F13" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>52560</v>
-      </c>
-      <c r="G13" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1011937.6800000002</v>
-      </c>
-      <c r="H13" s="2">
-        <f t="shared" ca="1" si="6"/>
-        <v>683280</v>
+      <c r="B13" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.11</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" ca="1" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" ca="1" si="4"/>
+        <v>89517.564000000013</v>
+      </c>
+      <c r="F13" s="6">
+        <f t="shared" ca="1" si="5"/>
+        <v>66488.399999999994</v>
+      </c>
+      <c r="G13" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1342763.4600000002</v>
+      </c>
+      <c r="H13" s="6">
+        <f t="shared" ca="1" si="6"/>
+        <v>997325.99999999988</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14">
-        <f t="shared" ca="1" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="C14" s="4">
+      <c r="B14" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="C14" s="7">
         <f t="shared" ca="1" si="2"/>
         <v>0.15</v>
       </c>
-      <c r="D14">
-        <f t="shared" ca="1" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="E14">
-        <f t="shared" ca="1" si="4"/>
-        <v>36325.968000000008</v>
-      </c>
-      <c r="F14" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>36792</v>
-      </c>
-      <c r="G14" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>217955.80800000005</v>
-      </c>
-      <c r="H14" s="2">
-        <f t="shared" ca="1" si="6"/>
-        <v>220752</v>
+      <c r="D14" s="5">
+        <f t="shared" ca="1" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" ca="1" si="4"/>
+        <v>29839.188000000002</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" ca="1" si="5"/>
+        <v>30221.999999999996</v>
+      </c>
+      <c r="G14" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>417748.63200000004</v>
+      </c>
+      <c r="H14" s="6">
+        <f t="shared" ca="1" si="6"/>
+        <v>423107.99999999994</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B15">
-        <f t="shared" ca="1" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="C15" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.15</v>
-      </c>
-      <c r="D15">
-        <f t="shared" ca="1" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="E15">
-        <f t="shared" ca="1" si="4"/>
-        <v>32433.9</v>
-      </c>
-      <c r="F15" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>32850</v>
-      </c>
-      <c r="G15" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>486508.5</v>
-      </c>
-      <c r="H15" s="2">
-        <f t="shared" ca="1" si="6"/>
-        <v>492750</v>
+      <c r="B15" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C15" s="7">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" ca="1" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" ca="1" si="4"/>
+        <v>10378.848</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" ca="1" si="5"/>
+        <v>7008</v>
+      </c>
+      <c r="G15" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>145303.872</v>
+      </c>
+      <c r="H15" s="6">
+        <f t="shared" ca="1" si="6"/>
+        <v>98112</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B16">
-        <f t="shared" ca="1" si="1"/>
-        <v>54</v>
-      </c>
-      <c r="C16" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.12</v>
-      </c>
-      <c r="D16">
-        <f t="shared" ca="1" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="E16">
-        <f t="shared" ca="1" si="4"/>
+      <c r="B16" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C16" s="7">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D16" s="5">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" ca="1" si="4"/>
+        <v>7784.1360000000004</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" ca="1" si="5"/>
+        <v>7358.4000000000005</v>
+      </c>
+      <c r="G16" s="6">
+        <f t="shared" ca="1" si="0"/>
         <v>70057.224000000002</v>
       </c>
-      <c r="F16" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>56764.799999999996</v>
-      </c>
-      <c r="G16" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>980801.13600000006</v>
-      </c>
-      <c r="H16" s="2">
-        <f t="shared" ca="1" si="6"/>
-        <v>794707.2</v>
+      <c r="H16" s="6">
+        <f t="shared" ca="1" si="6"/>
+        <v>66225.600000000006</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B17">
-        <f t="shared" ca="1" si="1"/>
-        <v>83</v>
-      </c>
-      <c r="C17" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.12</v>
-      </c>
-      <c r="D17">
-        <f t="shared" ca="1" si="3"/>
-        <v>13</v>
-      </c>
-      <c r="E17">
-        <f t="shared" ca="1" si="4"/>
-        <v>107680.54800000001</v>
-      </c>
-      <c r="F17" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>87249.599999999991</v>
-      </c>
-      <c r="G17" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1399847.1240000001</v>
-      </c>
-      <c r="H17" s="2">
-        <f t="shared" ca="1" si="6"/>
-        <v>1134244.7999999998</v>
+      <c r="B17" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="C17" s="7">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.15</v>
+      </c>
+      <c r="D17" s="5">
+        <f t="shared" ca="1" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" ca="1" si="4"/>
+        <v>89517.564000000013</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" ca="1" si="5"/>
+        <v>90666</v>
+      </c>
+      <c r="G17" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1253245.8960000002</v>
+      </c>
+      <c r="H17" s="6">
+        <f t="shared" ca="1" si="6"/>
+        <v>1269324</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E18">
         <f ca="1">SUM(E3:E17)</f>
-        <v>980801.13599999994</v>
+        <v>843281.40000000014</v>
       </c>
       <c r="F18" s="3">
         <f ca="1">SUM(F3:F17)</f>
-        <v>852435.6</v>
+        <v>753798.00000000012</v>
       </c>
       <c r="G18" s="2">
         <f ca="1">SUM(G3:G17)</f>
-        <v>11516629.211999999</v>
+        <v>9924773.3999999985</v>
       </c>
       <c r="H18" s="2">
         <f ca="1">SUM(H3:H17)</f>
-        <v>10097038.800000001</v>
+        <v>8713922.4000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>